<commit_message>
Last version before optimization
</commit_message>
<xml_diff>
--- a/ParseMusicEntries/finalized collections/spreadsheet outputs/sources.xlsx
+++ b/ParseMusicEntries/finalized collections/spreadsheet outputs/sources.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2690" uniqueCount="1672">
   <si>
-    <t>source_collection</t>
+    <t>collection_name</t>
   </si>
   <si>
     <t>source_number</t>
@@ -1888,7 +1888,7 @@
 		and 18 (occupied in this book by printed rudiments, and printed tunes whose 
 		titles don’t match) and between 108 and 151 (the pages in this book only go 
 		to p. 96), several tunes without page numbers (some of these appear in the 
-		book; others don’t), and other tunes that don't appear in this book (e.g., 
+		book; others don’t), and other tunes that don’t appear in this book (e.g., 
 		Russia, with a page number of 55 in the index, whereas in the MS. this is the 
 		second page of Scotland)</t>
   </si>
@@ -2874,7 +2874,7 @@
 		of the book, a. l. [1] verso is numbered 42, a. l. [2] recto is numbered 
 		43)
 	MS. music, all single vocal parts, appears to be all melodies (several entries 
-		marked “Air”); whether treble or tenor isn't known</t>
+		marked “Air”); whether treble or tenor isn’t known</t>
   </si>
   <si>
     <t>Quarto M 2116 .M23 C6 1809</t>
@@ -3317,7 +3317,7 @@
     <t>M 2116 .H5 S6</t>
   </si>
   <si>
-    <t>Solfeggio Americano[:] A System of Singing for the American Conservatorio with a variety of Psalmody suited to every metre.</t>
+    <t>Solfeggio :] A System of Singing for the American Conservatorio with a variety of Psalmody suited to every metre.</t>
   </si>
   <si>
     <t>preliminary leaf recto: “Charles T. Wells / from his friend / 
@@ -3928,7 +3928,7 @@
 		James [G?] Sewell”</t>
   </si>
   <si>
-    <t>2nd ed.]  Typeset pp. 3-[4], engraved pp. 1-[48] (leaf with pp. 47 + 48 is fragmentary, so p. nos. aren't present).  Pp. 29-32 printed + bound in this order (rectos/versos): 32/30, 31/29.  This tunebook comes closest to ASMI 354, except it has the signature of tunes paged 13-20 that is discussed in the 2nd full paragraph on p. 426 of ASMI.  The printed index on typeset p. [4] corresponds only partially to the musical content.  An early owner has listed the titles and p. nos. of the tunes on pp. 13-20 on the index page.
+    <t>2nd ed.]  Typeset pp. 3-[4], engraved pp. 1-[48] (leaf with pp. 47 + 48 is fragmentary, so p. nos. aren’t present).  Pp. 29-32 printed + bound in this order (rectos/versos): 32/30, 31/29.  This tunebook comes closest to ASMI 354, except it has the signature of tunes paged 13-20 that is discussed in the 2nd full paragraph on p. 426 of ASMI.  The printed index on typeset p. [4] corresponds only partially to the musical content.  An early owner has listed the titles and p. nos. of the tunes on pp. 13-20 on the index page.
 	text incipits supplied in MS. on pp. 5-11
 	no MS. music</t>
   </si>
@@ -4964,7 +4964,7 @@
     <t>Seymour, Lewis, and Thaddeus Seymour</t>
   </si>
   <si>
-    <t>The Musical Instructer: or An Easy Introduction to Psalmody.</t>
+    <t>The Musical Instructer: or  Easy Introduction to Psalmody.  2</t>
   </si>
   <si>
     <t>2nd ed.  New York, 1808.  [2], 5-53, [1] pp.  Complete.  Pp. 27-34 printed + bound in this order (rectos/versos): 27/32, 33/30, 31/28, 29/34.
@@ -5461,7 +5461,7 @@
 		one style to the other in the middle of a voice part, or from voice part 			to voice part in one entry
 	most entries lack bar lines, with only double bars to indicate the ends of 
 		phrases; consider all bar lines included here as literal transcriptions 
-		of what is and isn't present in the MS.</t>
+		of what is and isnt present in the MS.</t>
   </si>
   <si>
     <t>196</t>

</xml_diff>